<commit_message>
Edited Config and Test class for Vertical Booking
Change-Id: I13eb956a966d1d92c8d2f910b4b0d7ea1ca14807
Signed-off-by: Din Dayal Singh <din.dayal@hotelogix.com>
</commit_message>
<xml_diff>
--- a/ChannelAutomation/ChannelTestCases.xlsx
+++ b/ChannelAutomation/ChannelTestCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ChannelAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DD\ChannelAutomationRepo\ChannelAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ChannelSmokeTestCases" sheetId="1" r:id="rId1"/>
@@ -399,6 +399,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -436,6 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,11 +1126,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1592,7 +1594,11 @@
         <v>91</v>
       </c>
     </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Signed-off-by: Din Dayal Singh <din.dayal@hotelogix.com>
</commit_message>
<xml_diff>
--- a/ChannelAutomation/ChannelTestCases.xlsx
+++ b/ChannelAutomation/ChannelTestCases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChannelSmokeTestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="ChannelFunctionalTestCases" sheetId="2" r:id="rId2"/>
+    <sheet name="ChannelAllTestCases" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="114">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -394,13 +395,31 @@
   <si>
     <t>TC_38</t>
   </si>
+  <si>
+    <t>Logout Admin Console</t>
+  </si>
+  <si>
+    <t>1. Click on Logout link displaying at top-right corner</t>
+  </si>
+  <si>
+    <t>Admin Console should be logged out</t>
+  </si>
+  <si>
+    <t>Create Reservation on Frontdesk and Check Allotment Update</t>
+  </si>
+  <si>
+    <t>Cancel Reservation from Frontdesk and Check Allotment Update</t>
+  </si>
+  <si>
+    <t>Add DNR and Check Allotment Update</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -439,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,11 +772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,117 +1025,53 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1125,10 +1080,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1376,229 +1333,302 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE35848-3037-4A55-9C28-536DD3523A13}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>